<commit_message>
cronograma listo y asignacion de evento
</commit_message>
<xml_diff>
--- a/BO/Librería de Trabajo/Gestión de Proyecto/BO_C.xlsx
+++ b/BO/Librería de Trabajo/Gestión de Proyecto/BO_C.xlsx
@@ -531,7 +531,7 @@
   <dimension ref="C2:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +564,9 @@
       <c r="D5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="13">
+        <v>42490</v>
+      </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">

</xml_diff>